<commit_message>
cns infrastructure & cns capability SUR update
</commit_message>
<xml_diff>
--- a/data/cns_capability.xlsx
+++ b/data/cns_capability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482D58CA-2C33-4769-8A72-2F6875806F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A278BB7D-F256-46BB-889C-008E5FDF6EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="114">
   <si>
     <t>A – GBAS landing system</t>
   </si>
@@ -390,18 +390,12 @@
     <t>B737-800</t>
   </si>
   <si>
-    <t>DH8D</t>
-  </si>
-  <si>
     <t>B777-300ER</t>
   </si>
   <si>
     <t>CRJ9</t>
   </si>
   <si>
-    <t>A330-200</t>
-  </si>
-  <si>
     <t>ATR72-600</t>
   </si>
   <si>
@@ -409,6 +403,21 @@
   </si>
   <si>
     <t>E170</t>
+  </si>
+  <si>
+    <t>Palma de Mallorca</t>
+  </si>
+  <si>
+    <t>A321 NEO</t>
+  </si>
+  <si>
+    <t>B737 Max</t>
+  </si>
+  <si>
+    <t>B787 Dreamliner</t>
+  </si>
+  <si>
+    <t>ATR72-500</t>
   </si>
 </sst>
 </file>
@@ -457,8 +466,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,7 +841,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,10 +867,10 @@
         <v>66</v>
       </c>
       <c r="B2">
-        <v>4785926</v>
+        <v>4841403</v>
       </c>
       <c r="C2">
-        <v>0.43099999999999999</v>
+        <v>0.52300000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,10 +878,10 @@
         <v>67</v>
       </c>
       <c r="B3">
-        <v>2541601</v>
+        <v>1437964</v>
       </c>
       <c r="C3">
-        <v>0.22900000000000001</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,10 +889,10 @@
         <v>68</v>
       </c>
       <c r="B4">
-        <v>238086</v>
+        <v>274513</v>
       </c>
       <c r="C4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,10 +900,10 @@
         <v>69</v>
       </c>
       <c r="B5">
-        <v>3446300</v>
+        <v>2645524</v>
       </c>
       <c r="C5">
-        <v>0.31</v>
+        <v>0.28599999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,7 +911,7 @@
         <v>70</v>
       </c>
       <c r="B6">
-        <v>3493</v>
+        <v>2729</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -912,7 +922,7 @@
         <v>71</v>
       </c>
       <c r="B7">
-        <v>684</v>
+        <v>975</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -923,7 +933,7 @@
         <v>72</v>
       </c>
       <c r="B8">
-        <v>2148</v>
+        <v>3512</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -934,10 +944,10 @@
         <v>73</v>
       </c>
       <c r="B9">
-        <v>210661</v>
+        <v>122008</v>
       </c>
       <c r="C9">
-        <v>1.9E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,21 +955,21 @@
         <v>74</v>
       </c>
       <c r="B10">
-        <v>67066</v>
+        <v>88646</v>
       </c>
       <c r="C10">
-        <v>6.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B11">
-        <v>6069685</v>
+        <v>7409392</v>
       </c>
       <c r="C11">
-        <v>0.54700000000000004</v>
+        <v>0.80100000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,10 +977,10 @@
         <v>76</v>
       </c>
       <c r="B12">
-        <v>296965</v>
+        <v>329079</v>
       </c>
       <c r="C12">
-        <v>2.7E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -978,10 +988,10 @@
         <v>77</v>
       </c>
       <c r="B13">
-        <v>126493</v>
+        <v>44076</v>
       </c>
       <c r="C13">
-        <v>1.0999999999999999E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,10 +999,10 @@
         <v>78</v>
       </c>
       <c r="B14">
-        <v>17601</v>
+        <v>9195</v>
       </c>
       <c r="C14">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,10 +1010,10 @@
         <v>79</v>
       </c>
       <c r="B15">
-        <v>30667</v>
+        <v>64899</v>
       </c>
       <c r="C15">
-        <v>3.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,10 +1021,10 @@
         <v>80</v>
       </c>
       <c r="B16">
-        <v>19420</v>
+        <v>6092</v>
       </c>
       <c r="C16">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1030,7 +1040,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,34 +1082,34 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B2">
-        <v>0.34</v>
+        <v>0.877</v>
       </c>
       <c r="C2">
-        <v>0.54</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="D2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E2">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E2">
-        <v>0.11</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>6.0000000000000001E-3</v>
-      </c>
       <c r="J2">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1107,16 +1117,16 @@
         <v>91</v>
       </c>
       <c r="B3">
-        <v>0.69</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="C3">
-        <v>0.22</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="D3">
-        <v>2E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E3">
-        <v>0.09</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1128,10 +1138,10 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="J3">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1139,16 +1149,16 @@
         <v>92</v>
       </c>
       <c r="B4">
-        <v>0.42</v>
+        <v>0.53</v>
       </c>
       <c r="C4">
-        <v>0.48</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="D4">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E4">
-        <v>0.09</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1160,27 +1170,27 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>5.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="J4">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5">
-        <v>0.57999999999999996</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="C5">
-        <v>0.12</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="D5">
         <v>1.4E-2</v>
       </c>
       <c r="E5">
-        <v>0.28999999999999998</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1192,27 +1202,27 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>8.9999999999999993E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J5">
-        <v>0.02</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6">
-        <v>0.28999999999999998</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="C6">
-        <v>0.22</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="D6">
-        <v>3.3000000000000002E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E6">
-        <v>0.46</v>
+        <v>0.315</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1224,27 +1234,27 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>8.0000000000000002E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7">
-        <v>0.28999999999999998</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="C7">
-        <v>0.56999999999999995</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="D7">
-        <v>3.7999999999999999E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1256,10 +1266,10 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>8.9999999999999993E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="J7">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1267,16 +1277,16 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.28000000000000003</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="D8">
-        <v>1.2E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>0.61</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1288,27 +1298,27 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9">
-        <v>0.81</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="C9">
-        <v>0.11</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="D9">
-        <v>7.0000000000000001E-3</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E9">
-        <v>7.0000000000000007E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1320,42 +1330,42 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>4.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="B10">
-        <v>0.67</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="C10">
-        <v>0.11</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="D10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.317</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>2E-3</v>
+      </c>
+      <c r="J10">
         <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E10">
-        <v>0.21</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="J10">
-        <v>2E-3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1363,16 +1373,16 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.7</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="C11">
-        <v>0.04</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="D11">
-        <v>7.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E11">
-        <v>0.25</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1384,7 +1394,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1400,7 +1410,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G11"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,22 +1443,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B2">
-        <v>0.71499999999999997</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="C2">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="D2">
-        <v>6.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1459,22 +1469,22 @@
         <v>91</v>
       </c>
       <c r="B3">
-        <v>0.82</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="C3">
-        <v>0.01</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D3">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G3">
         <v>1E-3</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,42 +1492,42 @@
         <v>92</v>
       </c>
       <c r="B4">
-        <v>0.42499999999999999</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="C4">
-        <v>2.3E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D4">
-        <v>8.9999999999999993E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G4">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5">
-        <v>0.628</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="C5">
-        <v>5.7000000000000002E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D5">
-        <v>6.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1525,22 +1535,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6">
-        <v>0.50900000000000001</v>
+        <v>0.86099999999999999</v>
       </c>
       <c r="C6">
-        <v>3.1E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="D6">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>6.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1548,22 +1558,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7">
-        <v>0.55000000000000004</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="C7">
-        <v>3.9E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1E-3</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1574,42 +1584,42 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.56200000000000006</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="C8">
-        <v>2.1000000000000001E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D8">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G8">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9">
-        <v>0.79</v>
+        <v>0.872</v>
       </c>
       <c r="C9">
         <v>2.3E-2</v>
       </c>
       <c r="D9">
-        <v>8.0000000000000002E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1617,25 +1627,25 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="B10">
-        <v>0.77200000000000002</v>
+        <v>0.81</v>
       </c>
       <c r="C10">
-        <v>1.6E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D10">
-        <v>1.2E-2</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G10">
         <v>1E-3</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1643,19 +1653,19 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.73399999999999999</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="C11">
-        <v>2.5000000000000001E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D11">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1671,7 +1681,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,13 +1729,13 @@
         <v>0.46899999999999997</v>
       </c>
       <c r="C2">
-        <v>5.7000000000000002E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D2">
-        <v>7.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>0.46800000000000003</v>
+        <v>0.49</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1734,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1748,31 +1758,31 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>0.46100000000000002</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="C3">
-        <v>0.26200000000000001</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="D3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E3">
-        <v>0.26800000000000002</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1.4E-2</v>
-      </c>
-      <c r="J3">
-        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1780,16 +1790,16 @@
         <v>27</v>
       </c>
       <c r="B4">
-        <v>0.53300000000000003</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="C4">
-        <v>0.28399999999999997</v>
+        <v>0.28699999999999998</v>
       </c>
       <c r="D4">
-        <v>9.0999999999999998E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="E4">
-        <v>8.6999999999999994E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1804,24 +1814,24 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J4">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B5">
-        <v>0.495</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="C5">
-        <v>0.28399999999999997</v>
+        <v>0.121</v>
       </c>
       <c r="D5">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.218</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1833,27 +1843,27 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="B6">
-        <v>6.4000000000000001E-2</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="C6">
-        <v>0.75</v>
+        <v>0.253</v>
       </c>
       <c r="D6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.185</v>
+        <v>0.106</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1873,19 +1883,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="B7">
-        <v>0.31</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="C7">
-        <v>0.41899999999999998</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="D7">
-        <v>6.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E7">
-        <v>0.25800000000000001</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1897,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1905,19 +1915,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="B8">
-        <v>0.624</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="C8">
-        <v>0.159</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="D8">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E8">
-        <v>0.216</v>
+        <v>0.53</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1932,24 +1942,24 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.17799999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B9">
-        <v>0.81799999999999995</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="C9">
-        <v>5.7000000000000002E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E9">
-        <v>0.124</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1969,19 +1979,19 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="C10">
-        <v>0.88700000000000001</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="D10">
-        <v>1.4E-2</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>9.9000000000000005E-2</v>
+        <v>0.246</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -2001,19 +2011,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="B11">
-        <v>0.58399999999999996</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="C11">
-        <v>0.32400000000000001</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D11">
-        <v>3.5000000000000003E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E11">
-        <v>5.6000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -2033,19 +2043,19 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B12">
-        <v>0.71</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="C12">
-        <v>0.115</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D12">
-        <v>6.5000000000000002E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E12">
-        <v>0.109</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2065,19 +2075,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13">
-        <v>0.17699999999999999</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="C13">
-        <v>9.6000000000000002E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D13">
-        <v>0.254</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="E13">
-        <v>0.47099999999999997</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2097,19 +2107,19 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B14">
-        <v>0.81499999999999995</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="C14">
-        <v>0.125</v>
+        <v>0.16</v>
       </c>
       <c r="D14">
-        <v>7.0000000000000001E-3</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="E14">
-        <v>5.2999999999999999E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -2129,19 +2139,19 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B15">
-        <v>0.84499999999999997</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>5.0999999999999997E-2</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="D15">
-        <v>3.4000000000000002E-2</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="E15">
-        <v>6.9000000000000006E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2161,19 +2171,19 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B16">
-        <v>0.48899999999999999</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="C16">
-        <v>0.41899999999999998</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>8.2000000000000003E-2</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -2201,7 +2211,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,22 +2247,22 @@
         <v>103</v>
       </c>
       <c r="B2">
-        <v>0.86599999999999999</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="C2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D2">
-        <v>1.2999999999999999E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="E2">
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>2E-3</v>
       </c>
       <c r="G2">
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2260,22 +2270,22 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>0.498</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="C3">
-        <v>1.4E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D3">
-        <v>2.5999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>7.0000000000000001E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2283,10 +2293,10 @@
         <v>27</v>
       </c>
       <c r="B4">
-        <v>0.47</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="C4">
-        <v>9.0999999999999998E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2303,16 +2313,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B5">
-        <v>0.58699999999999997</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="C5">
-        <v>2E-3</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D5">
-        <v>4.2999999999999997E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2326,22 +2336,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="B6">
-        <v>6.6000000000000003E-2</v>
+        <v>0.91</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -2349,22 +2359,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="B7">
-        <v>0.54900000000000004</v>
+        <v>0.94099999999999995</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -2372,22 +2382,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="B8">
-        <v>0.93600000000000005</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="C8">
-        <v>8.9999999999999993E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -2395,13 +2405,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B9">
-        <v>0.94199999999999995</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="C9">
-        <v>2.3E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2418,13 +2428,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2441,10 +2451,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="B11">
-        <v>0.55900000000000005</v>
+        <v>0.996</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2464,22 +2474,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B12">
-        <v>0.79300000000000004</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="C12">
-        <v>2.5000000000000001E-2</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>1E-3</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -2487,13 +2497,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13">
-        <v>0.36</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2510,10 +2520,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B14">
-        <v>0.75700000000000001</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2522,24 +2532,24 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>1.9E-2</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B15">
-        <v>0.79700000000000004</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="C15">
-        <v>0.11899999999999999</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2556,10 +2566,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B16">
-        <v>0.48899999999999999</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="C16">
         <v>0</v>

</xml_diff>